<commit_message>
Core java Add two int and Array Sum division
</commit_message>
<xml_diff>
--- a/java/core-java/src/main/java/com/codejourney/core/doc/Core_Java_Complete_Topic_List.xlsx
+++ b/java/core-java/src/main/java/com/codejourney/core/doc/Core_Java_Complete_Topic_List.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2810" windowWidth="10700" windowHeight="4370"/>
+    <workbookView xWindow="0" yWindow="2810" windowWidth="10700" windowHeight="2840"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
     <sheet name="Core Java Topics" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
@@ -475,7 +475,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +487,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,17 +517,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3389,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3413,7 +3424,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3497,6 +3508,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>